<commit_message>
Fixed description storage in JSON
</commit_message>
<xml_diff>
--- a/Robocup/Robocup/downloads/russian_events.xlsx
+++ b/Robocup/Robocup/downloads/russian_events.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>One2113254766</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>One2684897887</t>
   </si>
   <si>
     <t xml:space="preserve"> adress</t>
@@ -28,6 +28,9 @@
     <t>date</t>
   </si>
   <si>
+    <t>desc</t>
+  </si>
+  <si>
     <t>name</t>
   </si>
   <si>
@@ -37,10 +40,13 @@
     <t>&lt;strong&gt;Адрес: &lt;/strong&gt;Adderss&lt;br&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt; &lt;li style="list-style-type: none;" &gt;                      &lt;a href="#" class="" style="padding: 0px" data-toggle="dropdown" role="button"                      aria-haspopup="true" aria-expanded="false"&gt;&lt;strong&gt;Инфо&lt;/strong&gt;                      &lt;span class="caret"&gt;&lt;/span&gt;&lt;/a&gt; &lt;ul class="dropdown-menu"&gt;                   &lt;li&gt;dfhxsn &lt;/li&gt;&lt;/ul&gt;                       &lt;/li&gt;                      &lt;strong&gt; Страна: &lt;/strong&gt;Россия&lt;br&gt;</t>
-  </si>
-  <si>
-    <t>&lt;strong&gt; Дата: 24-04-2020&lt;/strong&gt;&lt;/p&gt;</t>
+    <t>&lt;strong&gt; Страна: &lt;/strong&gt;Россия&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt; Дата: 21-04-2020&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; &lt;li style="list-style-type: none;" &gt;                      &lt;a href="#" class="" style="padding: 0px" data-toggle="dropdown" role="button"                      aria-haspopup="true" aria-expanded="false"&gt;&lt;strong&gt;Инфо&lt;/strong&gt;                      &lt;span class="caret"&gt;&lt;/span&gt;&lt;/a&gt; &lt;ul class="dropdown-menu"&gt;                   &lt;li&gt;description&lt;/li&gt;&lt;/ul&gt; &lt;/li&gt;</t>
   </si>
   <si>
     <t>&lt;h2&gt; One&lt;br&gt;&lt;strong&gt; Russian&lt;/strong&gt;&lt;/h2&gt;</t>
@@ -404,7 +410,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -420,7 +426,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -428,7 +434,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -436,7 +442,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -444,7 +450,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -452,7 +458,15 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>